<commit_message>
update new T- shit
</commit_message>
<xml_diff>
--- a/AmazonCreateTemplateFile/bin/Debug/zamage.com-1626882450.xlsx
+++ b/AmazonCreateTemplateFile/bin/Debug/zamage.com-1626882450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectDev\AmazonCreateTemplateFile\AmazonCreateTemplateFile\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01598F-C47E-4C83-AAE9-AD1D78628FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AFA483-E7D4-49F3-91FB-2D5550DE9347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,6 +418,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>